<commit_message>
FInalizado a distribuição das tarefas de programação
</commit_message>
<xml_diff>
--- a/Gestao_de_Projeto/listagem_de_tarefas_pendentes.xlsx
+++ b/Gestao_de_Projeto/listagem_de_tarefas_pendentes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t xml:space="preserve">Tipo</t>
   </si>
@@ -40,45 +40,45 @@
     <t xml:space="preserve">casos de uso</t>
   </si>
   <si>
+    <t xml:space="preserve">angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver classes para efetuar o login no frontend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efetuar login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bootstrap/html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver tela de login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listar vagas em aberto</t>
+  </si>
+  <si>
     <t xml:space="preserve">java</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver classes para efetuar login no backend</t>
   </si>
   <si>
-    <t xml:space="preserve">Anderson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">efetuar login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">angular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver classes para efetuar o login no frontend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">listar vagas em aberto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bootstrap/html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver tela de login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ok</t>
-  </si>
-  <si>
     <t xml:space="preserve">uc3</t>
   </si>
   <si>
@@ -88,6 +88,9 @@
     <t xml:space="preserve">Desenvolver classes para listar vagas, parecido com o de setores</t>
   </si>
   <si>
+    <t xml:space="preserve">Everton</t>
+  </si>
+  <si>
     <t xml:space="preserve">uc4</t>
   </si>
   <si>
@@ -103,76 +106,85 @@
     <t xml:space="preserve">criar vaga</t>
   </si>
   <si>
+    <t xml:space="preserve">Desenvolver classe ou método mostra a vaga selecionada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joziel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uc6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alterar vaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver tela para mostrar a vaga desejada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inativar vaga</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desenvolver classe ou método que efetua a ação de candidatar o usuário a vaga</t>
   </si>
   <si>
-    <t xml:space="preserve">uc6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alterar vaga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uc7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inativar vaga</t>
+    <t xml:space="preserve">uc8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizar Candidato</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver tela para confirmar a candidatura, ou utiliza a tela de visualizar vaga</t>
   </si>
   <si>
-    <t xml:space="preserve">uc8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizar Candidato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver tela para mostrar a vaga desejada</t>
-  </si>
-  <si>
     <t xml:space="preserve">uc9</t>
   </si>
   <si>
     <t xml:space="preserve">Alterar dados cadastrais</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver classe ou método mostra a vaga selecionada</t>
-  </si>
-  <si>
     <t xml:space="preserve">uc10</t>
   </si>
   <si>
     <t xml:space="preserve">Receber retorno vaga</t>
   </si>
   <si>
+    <t xml:space="preserve">Desenvolver classe para enviar dados da nova vaga ao java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernando</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desenvolver tela de fomulario para cadastrar vaga</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver classe para enviar dados da nova vaga ao java</t>
+    <t xml:space="preserve">Desenvolver classe para enviar dados da vaga editada ao java</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver tela de fomulario para alterar vaga, dica dá para usar o mesmo de cadastrar</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver classe para enviar dados da vaga editada ao java</t>
+    <t xml:space="preserve">Desenvolver classe ou método que altera o status da vaga e informa o backend</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver tela ou utilizar algum existente para colocar o botão de inativar vaga</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver classe ou método que altera o status da vaga e informa o backend</t>
+    <t xml:space="preserve">Desenvolver classe ou método mostra os dados do candidato inscrito na vaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alisson</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver tela que mostra os dados do candidato inscrito na vaga</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver classe ou método mostra os dados do candidato inscrito na vaga</t>
+    <t xml:space="preserve">Desenvolver classe ou método mostra os dados do candidato e envia os alterados para o  backend</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver tela que mostra os dados do candidato e um formulário para editar os dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolver classe ou método mostra os dados do candidato e envia os alterados para o  backend</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolver classes que enviem e-mail ao candidato quando a vaga for finalizada</t>
@@ -190,6 +202,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -278,7 +291,7 @@
   <dimension ref="B3:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -287,7 +300,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="81.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="1.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
@@ -325,52 +340,52 @@
       <c r="E4" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="H4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="H6" s="0" t="s">
         <v>19</v>
       </c>
@@ -380,7 +395,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2</v>
@@ -388,234 +403,288 @@
       <c r="D7" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>41</v>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>42</v>
+      <c r="D15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>43</v>
+      <c r="D16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>